<commit_message>
Update Data Dictionary - Capstone.xlsx
</commit_message>
<xml_diff>
--- a/Capstone/data/Data Dictionary - Capstone.xlsx
+++ b/Capstone/data/Data Dictionary - Capstone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnpicao\Documents\GitHub\batch3-workspace\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5359FB-592F-44CA-AA8B-B0FA99880E08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5024EFF-7CA8-45A8-A5AC-1780FD0C1AD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -689,7 +689,7 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -885,7 +885,7 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="7" t="s">

</xml_diff>